<commit_message>
[UPDATE] Enunciado y Ejemplos.
Se ha actualizado el enunciado de la practica, y se agregaron los ejemplos para que se visualice de mejor manera como seria el funcionamiento del display.
</commit_message>
<xml_diff>
--- a/Practica1/Practica1.xlsx
+++ b/Practica1/Practica1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\2025\Auxiliatura\Orga\EJEMPLOSORGA1S2025\Practica1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32F024-C56A-4287-B513-8047DA2881BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1000DB0-5FA0-4538-91C5-6FB3C399EED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{DCEB59B2-2147-42C9-800F-10DC07A93388}"/>
+    <workbookView xWindow="25440" yWindow="0" windowWidth="13065" windowHeight="15585" activeTab="1" xr2:uid="{DCEB59B2-2147-42C9-800F-10DC07A93388}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Entradas</t>
   </si>
@@ -130,12 +130,6 @@
     <t>1,0</t>
   </si>
   <si>
-    <t>(0,1)(0,0)+(0,1)(0,1)+(0,1)(1,1)+(0,1)(1,0)</t>
-  </si>
-  <si>
-    <t>W'X</t>
-  </si>
-  <si>
     <t>Minterminos</t>
   </si>
   <si>
@@ -145,30 +139,9 @@
     <t>WX</t>
   </si>
   <si>
-    <t>(1,0)(0,0)+(1,0)(0,1)+(1,0)(1,1)+(1,0)(1,0)</t>
-  </si>
-  <si>
     <t>YZ'</t>
   </si>
   <si>
-    <t>Resultado:</t>
-  </si>
-  <si>
-    <t>W'X+WX+YZ'</t>
-  </si>
-  <si>
-    <t>(A*B)+(A*B')= A</t>
-  </si>
-  <si>
-    <t>(W*X)+(W'*X)= X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simpli: </t>
-  </si>
-  <si>
-    <t>X+YZ'</t>
-  </si>
-  <si>
     <t>Maxterminos</t>
   </si>
   <si>
@@ -208,13 +181,43 @@
     <t>W'+X+Y'+Z'</t>
   </si>
   <si>
-    <t>(X)((W+Y+Z)(W+Y+Z')(W+Y'+Z')(W'+Y+Z)(W'+Y+Z')(W'+Y'+Z'))</t>
-  </si>
-  <si>
-    <t>f(W, X, Y, Z) = (X + Y)(X + Z')</t>
-  </si>
-  <si>
     <t>(0,1)(0,0)+(0,1)(0,1)+(1,1)(0,0)+(1,1)(0,1)</t>
+  </si>
+  <si>
+    <t>(0,0)(1,0)+(0,1)(1,0)+(1,1)(1,0)+(1,0)(1,0)</t>
+  </si>
+  <si>
+    <t>XY'</t>
+  </si>
+  <si>
+    <t>W'XY'Z'+W'XY'Z+WXY'Z'+WXY'Z</t>
+  </si>
+  <si>
+    <t>W'XY'+W'XY'+WXY'+WXY'</t>
+  </si>
+  <si>
+    <t>XY'+XY'+XY'+XY'</t>
+  </si>
+  <si>
+    <t>F(W,X,Y,Z)=</t>
+  </si>
+  <si>
+    <t>XY'+WX+YZ'</t>
+  </si>
+  <si>
+    <t>(0,1)(1,1)</t>
+  </si>
+  <si>
+    <t>W+X'+Y'+Z'</t>
+  </si>
+  <si>
+    <t>(X)((W+Y+Z)(W+Y+Z')(W+Y'+Z')(W'+Y+Z)(W'+Y+Z')(W'+Y'+Z')(W+X'+Y+Z'))</t>
+  </si>
+  <si>
+    <t>f(W, X, Y, Z) = (X + Y)(W + Y' + Z')(X + Z')</t>
+  </si>
+  <si>
+    <t>F(W, X, Y, Z) = (X + Y)(W + Y' + Z')(X + Z')</t>
   </si>
 </sst>
 </file>
@@ -248,12 +251,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -387,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -399,12 +444,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -414,13 +453,64 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -760,29 +850,29 @@
   <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:M19"/>
+      <selection activeCell="G3" sqref="G3:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="11" t="s">
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
       <c r="O2" t="s">
         <v>16</v>
       </c>
@@ -1543,22 +1633,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E222B1F1-1E9D-47E5-8B50-7CFB02FF7A54}">
-  <dimension ref="B2:M42"/>
+  <dimension ref="B2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:M6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1578,7 +1668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1600,20 +1690,20 @@
       <c r="I3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="32">
+        <v>0</v>
+      </c>
+      <c r="K3" s="34">
+        <v>0</v>
+      </c>
+      <c r="L3" s="35">
+        <v>0</v>
+      </c>
+      <c r="M3" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
@@ -1635,20 +1725,20 @@
       <c r="I4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J4" s="26">
+        <v>1</v>
+      </c>
+      <c r="K4" s="26">
+        <v>1</v>
+      </c>
+      <c r="L4" s="39">
+        <v>0</v>
+      </c>
+      <c r="M4" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1670,20 +1760,20 @@
       <c r="I5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J5" s="26">
+        <v>1</v>
+      </c>
+      <c r="K5" s="26">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27">
+        <v>1</v>
+      </c>
+      <c r="M5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -1705,40 +1795,40 @@
       <c r="I6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="J6" s="21">
+        <v>0</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="36">
+        <v>0</v>
+      </c>
+      <c r="M6" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="16">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16">
-        <v>0</v>
-      </c>
-      <c r="E7" s="16">
-        <v>1</v>
-      </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -1758,10 +1848,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>5</v>
       </c>
@@ -1780,14 +1870,14 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -1806,8 +1896,14 @@
       <c r="G10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
@@ -1826,8 +1922,14 @@
       <c r="G11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -1846,8 +1948,14 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -1866,8 +1974,14 @@
       <c r="G13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>10</v>
       </c>
@@ -1886,8 +2000,14 @@
       <c r="G14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I14" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>11</v>
       </c>
@@ -1906,8 +2026,14 @@
       <c r="G15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I15" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>12</v>
       </c>
@@ -1926,8 +2052,16 @@
       <c r="G16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>13</v>
       </c>
@@ -1946,8 +2080,15 @@
       <c r="G17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>14</v>
       </c>
@@ -1967,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1987,150 +2128,170 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="17">
+        <v>1</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>1</v>
+      </c>
+      <c r="F24" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F31" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="B36" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="I17:M17"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="I16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>